<commit_message>
Fix cells.AT-POS getting cell positions wrong
It is allowed to have missing cell nodes in the XML data. Thus accessing
them by position can miss the wanted cell. So we instead parse all cells
in a row when accessing the row the first time placing them in the correct
spot in the @!rows array. Gaps are filled with the Cell type object. This
makes sure later accesses to such gaps don't cause a re-processing of the
row.
</commit_message>
<xml_diff>
--- a/t/test-data/basic.xlsx
+++ b/t/test-data/basic.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.boeker\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14355" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Songs" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Song</t>
   </si>
@@ -24,9 +29,6 @@
   </si>
   <si>
     <t>Jinjer</t>
-  </si>
-  <si>
-    <t>Home Back</t>
   </si>
   <si>
     <t>Metalness</t>
@@ -74,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +119,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -125,12 +127,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -172,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -418,11 +423,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
@@ -437,26 +442,23 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -464,10 +466,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -483,11 +485,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -496,21 +498,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -518,10 +520,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -529,10 +531,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4">
         <v>9</v>

</xml_diff>